<commit_message>
Reformatted code, added dependecy list, Updated Query performance sheet
</commit_message>
<xml_diff>
--- a/Query_Performance.xlsx
+++ b/Query_Performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Python Workspace\Euclidean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Python Workspace\euclidean_distance_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="9">
   <si>
     <t>[</t>
   </si>
@@ -114,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -137,6 +137,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4470,10 +4474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K5"/>
+  <dimension ref="B3:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4555,7 +4559,6 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
       <c r="H5" s="8">
         <v>1.2275352000000299</v>
       </c>
@@ -4564,6 +4567,30 @@
         <v>40.214550600000599</v>
       </c>
       <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10">
+        <v>8.8003999999997903E-2</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.20115930000000001</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.32534079999999199</v>
+      </c>
+      <c r="J6" s="11">
+        <v>17.4160189000001</v>
+      </c>
+      <c r="K6" s="11">
+        <v>64.9894745000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added load tesing modules with multiprocessing and threading for testing perfromance
</commit_message>
<xml_diff>
--- a/Query_Performance.xlsx
+++ b/Query_Performance.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="12">
   <si>
     <t>[</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Solr</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>SolrCloud</t>
+  </si>
+  <si>
+    <t>Standalone</t>
   </si>
 </sst>
 </file>
@@ -114,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -141,6 +150,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4474,10 +4484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K6"/>
+  <dimension ref="B3:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4485,9 +4495,10 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -4518,8 +4529,11 @@
       <c r="K3" s="4">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -4550,8 +4564,9 @@
       <c r="K4" s="5">
         <v>83.830061599999894</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
@@ -4567,8 +4582,11 @@
         <v>40.214550600000599</v>
       </c>
       <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
@@ -4576,20 +4594,23 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="10">
+      <c r="G6" s="6">
         <v>8.8003999999997903E-2</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="12">
         <v>0.20115930000000001</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="12">
         <v>0.32534079999999199</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>17.4160189000001</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="8">
         <v>64.9894745000001</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>